<commit_message>
0.9 Domoticz relay state update
</commit_message>
<xml_diff>
--- a/docs/flash-map/flash-map.xlsx
+++ b/docs/flash-map/flash-map.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -37,12 +37,6 @@
     <t>WIFI SSID</t>
   </si>
   <si>
-    <t>MQTT Host</t>
-  </si>
-  <si>
-    <t>MQTT Port</t>
-  </si>
-  <si>
     <t>MQTT User</t>
   </si>
   <si>
@@ -116,6 +110,18 @@
   </si>
   <si>
     <t>Duration between next series of connection attempts (WiFi,MQTT)</t>
+  </si>
+  <si>
+    <t>Domoticz IDX</t>
+  </si>
+  <si>
+    <t>MQTT Host / Domoticz Host</t>
+  </si>
+  <si>
+    <t>MQTT Port / Domoticz Port</t>
+  </si>
+  <si>
+    <t>Publish relay state to Domoticz</t>
   </si>
 </sst>
 </file>
@@ -148,7 +154,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,6 +170,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -196,7 +208,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -208,6 +220,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
@@ -515,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +568,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" s="4">
         <v>96</v>
@@ -571,7 +584,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
@@ -587,7 +600,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2">
         <v>5</v>
@@ -603,7 +616,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2">
         <v>8</v>
@@ -619,7 +632,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
@@ -635,7 +648,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2">
         <v>6</v>
@@ -651,13 +664,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" ref="C9:C14" si="6">D8+1</f>
+        <f t="shared" ref="C9:C13" si="6">D8+1</f>
         <v>125</v>
       </c>
       <c r="D9" s="2">
@@ -667,7 +680,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
@@ -683,7 +696,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="2">
         <v>2</v>
@@ -699,7 +712,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
@@ -715,7 +728,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" s="2">
         <v>1</v>
@@ -731,7 +744,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2">
         <v>1</v>
@@ -747,7 +760,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15" s="2">
         <v>2</v>
@@ -761,12 +774,12 @@
         <v>133</v>
       </c>
       <c r="E15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" s="2">
         <v>2</v>
@@ -780,12 +793,12 @@
         <v>135</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B17" s="6">
         <v>2</v>
@@ -799,12 +812,12 @@
         <v>137</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18" s="2">
         <v>1</v>
@@ -820,7 +833,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>1</v>
@@ -836,7 +849,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2">
         <v>2</v>
@@ -852,7 +865,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B21" s="2">
         <v>32</v>
@@ -868,7 +881,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B22" s="4">
         <v>58</v>
@@ -919,7 +932,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B25" s="2">
         <v>32</v>
@@ -935,7 +948,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="B26" s="2">
         <v>5</v>
@@ -951,7 +964,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B27" s="2">
         <v>32</v>
@@ -967,7 +980,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B28" s="2">
         <v>32</v>
@@ -984,7 +997,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B29" s="2">
         <v>32</v>
@@ -999,43 +1012,51 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="4">
+      <c r="A30" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="4">
+      <c r="B30" s="7">
+        <v>3</v>
+      </c>
+      <c r="C30" s="7">
         <f t="shared" si="10"/>
         <v>429</v>
       </c>
-      <c r="D30" s="4">
-        <f t="shared" si="11"/>
-        <v>460</v>
+      <c r="D30" s="7">
+        <f t="shared" si="11"/>
+        <v>431</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2">
-        <f t="shared" si="10"/>
-        <v>461</v>
-      </c>
-      <c r="D31" s="2">
-        <f t="shared" si="11"/>
-        <v>460</v>
+      <c r="A31" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="6">
+        <v>1</v>
+      </c>
+      <c r="C31" s="6">
+        <f t="shared" si="10"/>
+        <v>432</v>
+      </c>
+      <c r="D31" s="6">
+        <f t="shared" si="11"/>
+        <v>432</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2">
-        <f t="shared" si="10"/>
-        <v>461</v>
-      </c>
-      <c r="D32" s="2">
-        <f t="shared" si="11"/>
-        <v>460</v>
+      <c r="A32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="4">
+        <v>80</v>
+      </c>
+      <c r="C32" s="4">
+        <f t="shared" si="10"/>
+        <v>433</v>
+      </c>
+      <c r="D32" s="4">
+        <f t="shared" si="11"/>
+        <v>512</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1043,11 +1064,11 @@
       <c r="B33" s="2"/>
       <c r="C33" s="2">
         <f t="shared" si="10"/>
-        <v>461</v>
+        <v>513</v>
       </c>
       <c r="D33" s="2">
         <f t="shared" si="11"/>
-        <v>460</v>
+        <v>512</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1055,11 +1076,11 @@
       <c r="B34" s="2"/>
       <c r="C34" s="2">
         <f t="shared" si="10"/>
-        <v>461</v>
+        <v>513</v>
       </c>
       <c r="D34" s="2">
         <f t="shared" si="11"/>
-        <v>460</v>
+        <v>512</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1067,11 +1088,11 @@
       <c r="B35" s="2"/>
       <c r="C35" s="2">
         <f t="shared" si="10"/>
-        <v>461</v>
+        <v>513</v>
       </c>
       <c r="D35" s="2">
         <f t="shared" si="11"/>
-        <v>460</v>
+        <v>512</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1079,11 +1100,11 @@
       <c r="B36" s="2"/>
       <c r="C36" s="2">
         <f t="shared" si="10"/>
-        <v>461</v>
+        <v>513</v>
       </c>
       <c r="D36" s="2">
         <f t="shared" si="11"/>
-        <v>460</v>
+        <v>512</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1091,11 +1112,11 @@
       <c r="B37" s="2"/>
       <c r="C37" s="2">
         <f t="shared" si="10"/>
-        <v>461</v>
+        <v>513</v>
       </c>
       <c r="D37" s="2">
         <f t="shared" si="11"/>
-        <v>460</v>
+        <v>512</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1103,11 +1124,11 @@
       <c r="B38" s="2"/>
       <c r="C38" s="2">
         <f t="shared" si="10"/>
-        <v>461</v>
+        <v>513</v>
       </c>
       <c r="D38" s="2">
         <f t="shared" si="11"/>
-        <v>460</v>
+        <v>512</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1115,11 +1136,11 @@
       <c r="B39" s="2"/>
       <c r="C39" s="2">
         <f t="shared" si="10"/>
-        <v>461</v>
+        <v>513</v>
       </c>
       <c r="D39" s="2">
         <f t="shared" si="11"/>
-        <v>460</v>
+        <v>512</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1127,11 +1148,11 @@
       <c r="B40" s="2"/>
       <c r="C40" s="2">
         <f t="shared" si="10"/>
-        <v>461</v>
+        <v>513</v>
       </c>
       <c r="D40" s="2">
         <f t="shared" si="11"/>
-        <v>460</v>
+        <v>512</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1139,11 +1160,11 @@
       <c r="B41" s="2"/>
       <c r="C41" s="2">
         <f t="shared" si="10"/>
-        <v>461</v>
+        <v>513</v>
       </c>
       <c r="D41" s="2">
         <f t="shared" si="11"/>
-        <v>460</v>
+        <v>512</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1151,11 +1172,11 @@
       <c r="B42" s="2"/>
       <c r="C42" s="2">
         <f t="shared" si="10"/>
-        <v>461</v>
+        <v>513</v>
       </c>
       <c r="D42" s="2">
         <f t="shared" si="11"/>
-        <v>460</v>
+        <v>512</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1163,11 +1184,11 @@
       <c r="B43" s="2"/>
       <c r="C43" s="2">
         <f t="shared" si="10"/>
-        <v>461</v>
+        <v>513</v>
       </c>
       <c r="D43" s="2">
         <f t="shared" si="11"/>
-        <v>460</v>
+        <v>512</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1175,11 +1196,11 @@
       <c r="B44" s="2"/>
       <c r="C44" s="2">
         <f t="shared" si="10"/>
-        <v>461</v>
+        <v>513</v>
       </c>
       <c r="D44" s="2">
         <f t="shared" si="11"/>
-        <v>460</v>
+        <v>512</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1187,11 +1208,11 @@
       <c r="B45" s="2"/>
       <c r="C45" s="2">
         <f t="shared" si="10"/>
-        <v>461</v>
+        <v>513</v>
       </c>
       <c r="D45" s="2">
         <f t="shared" si="11"/>
-        <v>460</v>
+        <v>512</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0.8.9 Added switch selection type (bistable/monostable) to the Sonoff configuration page.
</commit_message>
<xml_diff>
--- a/docs/flash-map/flash-map.xlsx
+++ b/docs/flash-map/flash-map.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -122,13 +122,16 @@
   </si>
   <si>
     <t>Publish relay state to Domoticz</t>
+  </si>
+  <si>
+    <t>Switch Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,7 +285,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -314,10 +317,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -349,7 +351,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -525,19 +526,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="59.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +552,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -566,7 +567,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -582,7 +583,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -598,7 +599,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -614,7 +615,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -630,7 +631,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -642,11 +643,11 @@
         <v>118</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" ref="D7:D23" si="4">B7+C7-1</f>
+        <f t="shared" ref="D7:D24" si="4">B7+C7-1</f>
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -654,7 +655,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" ref="C8:C22" si="5">D7+1</f>
+        <f t="shared" ref="C8:C21" si="5">D7+1</f>
         <v>119</v>
       </c>
       <c r="D8" s="2">
@@ -662,7 +663,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -678,7 +679,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -694,7 +695,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -710,7 +711,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
@@ -726,7 +727,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="5" t="s">
         <v>24</v>
       </c>
@@ -742,7 +743,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="5" t="s">
         <v>25</v>
       </c>
@@ -758,7 +759,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="5" t="s">
         <v>29</v>
       </c>
@@ -777,7 +778,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="5" t="s">
         <v>30</v>
       </c>
@@ -796,7 +797,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="6" t="s">
         <v>31</v>
       </c>
@@ -815,7 +816,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -831,7 +832,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -847,7 +848,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -863,7 +864,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="2" t="s">
         <v>13</v>
       </c>
@@ -879,199 +880,200 @@
         <v>173</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:10">
+      <c r="A22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2">
+        <v>174</v>
+      </c>
+      <c r="D22" s="2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="4">
-        <v>58</v>
-      </c>
-      <c r="C22" s="4">
-        <f t="shared" si="5"/>
-        <v>174</v>
-      </c>
-      <c r="D22" s="4">
+      <c r="B23" s="4">
+        <v>56</v>
+      </c>
+      <c r="C23" s="4">
+        <v>176</v>
+      </c>
+      <c r="D23" s="4">
         <f t="shared" si="4"/>
         <v>231</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+    <row r="24" spans="1:10">
+      <c r="A24" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B24" s="2">
         <v>32</v>
       </c>
-      <c r="C23" s="2">
-        <f t="shared" ref="C23:C45" si="10">D22+1</f>
+      <c r="C24" s="2">
+        <f t="shared" ref="C24:C46" si="10">D23+1</f>
         <v>232</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D24" s="2">
         <f t="shared" si="4"/>
         <v>263</v>
       </c>
-      <c r="F23">
+      <c r="F24">
         <v>232</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+    <row r="25" spans="1:10">
+      <c r="A25" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="B24" s="2">
-        <v>32</v>
-      </c>
-      <c r="C24" s="2">
-        <f t="shared" si="10"/>
-        <v>264</v>
-      </c>
-      <c r="D24" s="2">
-        <f t="shared" ref="D24:D45" si="11">B24+C24-1</f>
-        <v>295</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="B25" s="2">
         <v>32</v>
       </c>
       <c r="C25" s="2">
         <f t="shared" si="10"/>
+        <v>264</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" ref="D25:D46" si="11">B25+C25-1</f>
+        <v>295</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="2">
+        <v>32</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" si="10"/>
         <v>296</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D26" s="2">
         <f t="shared" si="11"/>
         <v>327</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+    <row r="27" spans="1:10">
+      <c r="A27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B27" s="2">
         <v>5</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C27" s="2">
         <f t="shared" si="10"/>
         <v>328</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D27" s="2">
         <f t="shared" si="11"/>
         <v>332</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    <row r="28" spans="1:10">
+      <c r="A28" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B27" s="2">
-        <v>32</v>
-      </c>
-      <c r="C27" s="2">
-        <f t="shared" si="10"/>
-        <v>333</v>
-      </c>
-      <c r="D27" s="2">
-        <f t="shared" si="11"/>
-        <v>364</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="B28" s="2">
         <v>32</v>
       </c>
       <c r="C28" s="2">
         <f t="shared" si="10"/>
-        <v>365</v>
+        <v>333</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" si="11"/>
-        <v>396</v>
-      </c>
-      <c r="J28" s="3"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B29" s="2">
         <v>32</v>
       </c>
       <c r="C29" s="2">
         <f t="shared" si="10"/>
+        <v>365</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="11"/>
+        <v>396</v>
+      </c>
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="2">
+        <v>32</v>
+      </c>
+      <c r="C30" s="2">
+        <f t="shared" si="10"/>
         <v>397</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D30" s="2">
         <f t="shared" si="11"/>
         <v>428</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+    <row r="31" spans="1:10">
+      <c r="A31" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B31" s="7">
         <v>3</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C31" s="7">
         <f t="shared" si="10"/>
         <v>429</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D31" s="7">
         <f t="shared" si="11"/>
         <v>431</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+    <row r="32" spans="1:10">
+      <c r="A32" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B32" s="6">
         <v>1</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C32" s="6">
         <f t="shared" si="10"/>
         <v>432</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D32" s="6">
         <f t="shared" si="11"/>
         <v>432</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+    <row r="33" spans="1:4">
+      <c r="A33" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B33" s="4">
         <v>80</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C33" s="4">
         <f t="shared" si="10"/>
         <v>433</v>
       </c>
-      <c r="D32" s="4">
-        <f t="shared" si="11"/>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2">
-        <f t="shared" si="10"/>
-        <v>513</v>
-      </c>
-      <c r="D33" s="2">
-        <f t="shared" si="11"/>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="4">
+        <f t="shared" si="11"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2">
@@ -1083,7 +1085,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2">
@@ -1095,7 +1097,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2">
@@ -1107,7 +1109,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2">
@@ -1119,7 +1121,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2">
@@ -1131,7 +1133,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2">
@@ -1143,7 +1145,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2">
@@ -1155,7 +1157,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2">
@@ -1167,7 +1169,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2">
@@ -1179,7 +1181,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2">
@@ -1191,7 +1193,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2">
@@ -1203,7 +1205,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2">
@@ -1211,6 +1213,18 @@
         <v>513</v>
       </c>
       <c r="D45" s="2">
+        <f t="shared" si="11"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2">
+        <f t="shared" si="10"/>
+        <v>513</v>
+      </c>
+      <c r="D46" s="2">
         <f t="shared" si="11"/>
         <v>512</v>
       </c>

</xml_diff>

<commit_message>
Added auto-off functionality with user defined timeout.
</commit_message>
<xml_diff>
--- a/docs/flash-map/flash-map.xlsx
+++ b/docs/flash-map/flash-map.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>Switch Type</t>
+  </si>
+  <si>
+    <t>Relay auto OFF time</t>
+  </si>
+  <si>
+    <t>0-99999s</t>
   </si>
 </sst>
 </file>
@@ -527,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -643,7 +649,7 @@
         <v>118</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" ref="D7:D24" si="4">B7+C7-1</f>
+        <f t="shared" ref="D7:D25" si="4">B7+C7-1</f>
         <v>118</v>
       </c>
     </row>
@@ -895,192 +901,194 @@
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="2">
+        <v>5</v>
+      </c>
+      <c r="C23" s="2">
+        <v>176</v>
+      </c>
+      <c r="D23" s="2">
+        <v>180</v>
+      </c>
+      <c r="E23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="4">
-        <v>56</v>
-      </c>
-      <c r="C23" s="4">
-        <v>176</v>
-      </c>
-      <c r="D23" s="4">
+      <c r="B24" s="4">
+        <v>51</v>
+      </c>
+      <c r="C24" s="4">
+        <v>181</v>
+      </c>
+      <c r="D24" s="4">
         <f t="shared" si="4"/>
         <v>231</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="2" t="s">
+    <row r="25" spans="1:10">
+      <c r="A25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B25" s="2">
         <v>32</v>
       </c>
-      <c r="C24" s="2">
-        <f t="shared" ref="C24:C46" si="10">D23+1</f>
+      <c r="C25" s="2">
+        <f t="shared" ref="C25:C47" si="10">D24+1</f>
         <v>232</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D25" s="2">
         <f t="shared" si="4"/>
         <v>263</v>
       </c>
-      <c r="F24">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="2">
-        <v>32</v>
-      </c>
-      <c r="C25" s="2">
-        <f t="shared" si="10"/>
-        <v>264</v>
-      </c>
-      <c r="D25" s="2">
-        <f t="shared" ref="D25:D46" si="11">B25+C25-1</f>
-        <v>295</v>
-      </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="2" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="B26" s="2">
         <v>32</v>
       </c>
       <c r="C26" s="2">
         <f t="shared" si="10"/>
-        <v>296</v>
+        <v>264</v>
       </c>
       <c r="D26" s="2">
-        <f t="shared" si="11"/>
-        <v>327</v>
+        <f t="shared" ref="D26:D47" si="11">B26+C26-1</f>
+        <v>295</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="2">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C27" s="2">
         <f t="shared" si="10"/>
-        <v>328</v>
+        <v>296</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="11"/>
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="2" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="B28" s="2">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="C28" s="2">
         <f t="shared" si="10"/>
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" si="11"/>
-        <v>364</v>
+        <v>332</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B29" s="2">
         <v>32</v>
       </c>
       <c r="C29" s="2">
         <f t="shared" si="10"/>
-        <v>365</v>
+        <v>333</v>
       </c>
       <c r="D29" s="2">
         <f t="shared" si="11"/>
-        <v>396</v>
-      </c>
-      <c r="J29" s="3"/>
+        <v>364</v>
+      </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B30" s="2">
         <v>32</v>
       </c>
       <c r="C30" s="2">
         <f t="shared" si="10"/>
+        <v>365</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="11"/>
+        <v>396</v>
+      </c>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="2">
+        <v>32</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="10"/>
         <v>397</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D31" s="2">
         <f t="shared" si="11"/>
         <v>428</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="7" t="s">
+    <row r="32" spans="1:10">
+      <c r="A32" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B32" s="7">
         <v>3</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C32" s="7">
         <f t="shared" si="10"/>
         <v>429</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D32" s="7">
         <f t="shared" si="11"/>
         <v>431</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="6" t="s">
+    <row r="33" spans="1:4">
+      <c r="A33" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B33" s="6">
         <v>1</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C33" s="6">
         <f t="shared" si="10"/>
         <v>432</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D33" s="6">
         <f t="shared" si="11"/>
         <v>432</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="4" t="s">
+    <row r="34" spans="1:4">
+      <c r="A34" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B34" s="4">
         <v>80</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C34" s="4">
         <f t="shared" si="10"/>
         <v>433</v>
       </c>
-      <c r="D33" s="4">
-        <f t="shared" si="11"/>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2">
-        <f t="shared" si="10"/>
-        <v>513</v>
-      </c>
-      <c r="D34" s="2">
+      <c r="D34" s="4">
         <f t="shared" si="11"/>
         <v>512</v>
       </c>
@@ -1225,6 +1233,18 @@
         <v>513</v>
       </c>
       <c r="D46" s="2">
+        <f t="shared" si="11"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2">
+        <f t="shared" si="10"/>
+        <v>513</v>
+      </c>
+      <c r="D47" s="2">
         <f t="shared" si="11"/>
         <v>512</v>
       </c>

</xml_diff>

<commit_message>
added static IP - no testing
</commit_message>
<xml_diff>
--- a/docs/flash-map/flash-map.xlsx
+++ b/docs/flash-map/flash-map.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -125,13 +125,22 @@
   </si>
   <si>
     <t>Switch Type</t>
+  </si>
+  <si>
+    <t>Static IP</t>
+  </si>
+  <si>
+    <t>Static subnet mask</t>
+  </si>
+  <si>
+    <t>Static gateway</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,7 +294,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -317,9 +326,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -351,6 +361,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -526,19 +537,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -552,7 +563,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -567,665 +578,713 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="2">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2">
+        <f t="shared" ref="C3:C6" si="0">D2+1</f>
+        <v>8</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" ref="D3:D6" si="1">B3+C3-1</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="2">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B3" s="4">
-        <v>96</v>
-      </c>
-      <c r="C3" s="4">
-        <f>D2+1</f>
-        <v>8</v>
-      </c>
-      <c r="D3" s="4">
-        <f>B3+C3-1</f>
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="2" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4">
+        <v>81</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2">
-        <f t="shared" ref="C4" si="0">D3+1</f>
-        <v>104</v>
-      </c>
-      <c r="D4" s="2">
-        <f t="shared" ref="D4" si="1">B4+C4-1</f>
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="2">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2">
-        <f t="shared" ref="C5:C6" si="2">D4+1</f>
-        <v>105</v>
-      </c>
-      <c r="D5" s="2">
-        <f t="shared" ref="D5:D6" si="3">B5+C5-1</f>
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="2">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2">
-        <f t="shared" si="2"/>
-        <v>110</v>
-      </c>
-      <c r="D6" s="2">
-        <f t="shared" si="3"/>
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
       </c>
       <c r="C7" s="2">
-        <f>D6+1</f>
-        <v>118</v>
+        <f t="shared" ref="C7" si="2">D6+1</f>
+        <v>101</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" ref="D7:D24" si="4">B7+C7-1</f>
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <f t="shared" ref="D7" si="3">B7+C7-1</f>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" ref="C8:C21" si="5">D7+1</f>
-        <v>119</v>
+        <f t="shared" ref="C8:C9" si="4">D7+1</f>
+        <v>102</v>
       </c>
       <c r="D8" s="2">
+        <f t="shared" ref="D8:D9" si="5">B8+C8-1</f>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2">
         <f t="shared" si="4"/>
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2">
-        <f t="shared" ref="C9:C13" si="6">D8+1</f>
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" ref="D9:D13" si="7">B9+C9-1</f>
-        <v>125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <f t="shared" si="5"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
       </c>
       <c r="C10" s="2">
+        <f>D9+1</f>
+        <v>115</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" ref="D10:D27" si="6">B10+C10-1</f>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" ref="C11:C24" si="7">D10+1</f>
+        <v>116</v>
+      </c>
+      <c r="D11" s="2">
         <f t="shared" si="6"/>
-        <v>126</v>
-      </c>
-      <c r="D10" s="2">
-        <f t="shared" si="7"/>
-        <v>126</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="2">
-        <v>2</v>
-      </c>
-      <c r="C11" s="2">
-        <f t="shared" si="6"/>
-        <v>127</v>
-      </c>
-      <c r="D11" s="2">
-        <f t="shared" si="7"/>
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="5" t="s">
-        <v>23</v>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
       </c>
       <c r="C12" s="2">
-        <f t="shared" si="6"/>
-        <v>129</v>
+        <f t="shared" ref="C12:C16" si="8">D11+1</f>
+        <v>122</v>
       </c>
       <c r="D12" s="2">
-        <f t="shared" si="7"/>
-        <v>129</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="5" t="s">
-        <v>24</v>
+        <f t="shared" ref="D12:D16" si="9">B12+C12-1</f>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="B13" s="2">
         <v>1</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" si="6"/>
-        <v>130</v>
+        <f t="shared" si="8"/>
+        <v>123</v>
       </c>
       <c r="D13" s="2">
-        <f t="shared" si="7"/>
-        <v>130</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="5" t="s">
-        <v>25</v>
+        <f t="shared" si="9"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B14" s="2">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="8"/>
+        <v>124</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="9"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="2">
         <v>1</v>
       </c>
-      <c r="C14" s="2">
-        <f>D13+1</f>
-        <v>131</v>
-      </c>
-      <c r="D14" s="2">
-        <f>B14+C14-1</f>
-        <v>131</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="2">
-        <v>2</v>
-      </c>
       <c r="C15" s="2">
-        <f t="shared" ref="C15:C17" si="8">D14+1</f>
-        <v>132</v>
+        <f t="shared" si="8"/>
+        <v>126</v>
       </c>
       <c r="D15" s="2">
-        <f t="shared" ref="D15:D17" si="9">B15+C15-1</f>
-        <v>133</v>
-      </c>
-      <c r="E15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <f t="shared" si="9"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B16" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" si="8"/>
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="9"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2">
+        <f>D16+1</f>
+        <v>128</v>
+      </c>
+      <c r="D17" s="2">
+        <f>B17+C17-1</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" ref="C18:C20" si="10">D17+1</f>
+        <v>129</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" ref="D18:D20" si="11">B18+C18-1</f>
+        <v>130</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="10"/>
+        <v>131</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="11"/>
+        <v>132</v>
+      </c>
+      <c r="E19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="6">
+        <v>2</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="10"/>
+        <v>133</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="11"/>
+        <v>134</v>
+      </c>
+      <c r="E20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <f t="shared" si="7"/>
         <v>135</v>
       </c>
-      <c r="E16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="6">
+      <c r="D21" s="2">
+        <f t="shared" si="6"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2">
+        <f t="shared" si="7"/>
+        <v>136</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" si="6"/>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="2">
         <v>2</v>
       </c>
-      <c r="C17" s="2">
-        <f t="shared" si="8"/>
-        <v>136</v>
-      </c>
-      <c r="D17" s="2">
-        <f t="shared" si="9"/>
+      <c r="C23" s="2">
+        <f t="shared" si="7"/>
         <v>137</v>
       </c>
-      <c r="E17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="2">
-        <v>1</v>
-      </c>
-      <c r="C18" s="2">
-        <f t="shared" si="5"/>
+      <c r="D23" s="2">
+        <f t="shared" si="6"/>
         <v>138</v>
       </c>
-      <c r="D18" s="2">
-        <f t="shared" si="4"/>
-        <v>138</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2">
-        <v>1</v>
-      </c>
-      <c r="C19" s="2">
-        <f t="shared" si="5"/>
-        <v>139</v>
-      </c>
-      <c r="D19" s="2">
-        <f t="shared" si="4"/>
-        <v>139</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="2">
-        <v>2</v>
-      </c>
-      <c r="C20" s="2">
-        <f t="shared" si="5"/>
-        <v>140</v>
-      </c>
-      <c r="D20" s="2">
-        <f t="shared" si="4"/>
-        <v>141</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="2" t="s">
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B21" s="2">
-        <v>32</v>
-      </c>
-      <c r="C21" s="2">
-        <f t="shared" si="5"/>
-        <v>142</v>
-      </c>
-      <c r="D21" s="2">
-        <f t="shared" si="4"/>
-        <v>173</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="2">
-        <v>2</v>
-      </c>
-      <c r="C22" s="2">
-        <v>174</v>
-      </c>
-      <c r="D22" s="2">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="4">
-        <v>56</v>
-      </c>
-      <c r="C23" s="4">
-        <v>176</v>
-      </c>
-      <c r="D23" s="4">
-        <f t="shared" si="4"/>
-        <v>231</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="B24" s="2">
         <v>32</v>
       </c>
       <c r="C24" s="2">
-        <f t="shared" ref="C24:C46" si="10">D23+1</f>
+        <f t="shared" si="7"/>
+        <v>139</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" si="6"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2</v>
+      </c>
+      <c r="C25" s="2">
+        <v>174</v>
+      </c>
+      <c r="D25" s="2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="4">
+        <v>56</v>
+      </c>
+      <c r="C26" s="4">
+        <v>176</v>
+      </c>
+      <c r="D26" s="4">
+        <f t="shared" si="6"/>
+        <v>231</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2">
+        <v>32</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" ref="C27:C49" si="12">D26+1</f>
         <v>232</v>
       </c>
-      <c r="D24" s="2">
-        <f t="shared" si="4"/>
+      <c r="D27" s="2">
+        <f t="shared" si="6"/>
         <v>263</v>
       </c>
-      <c r="F24">
+      <c r="F27">
         <v>232</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="2" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="B25" s="2">
-        <v>32</v>
-      </c>
-      <c r="C25" s="2">
-        <f t="shared" si="10"/>
-        <v>264</v>
-      </c>
-      <c r="D25" s="2">
-        <f t="shared" ref="D25:D46" si="11">B25+C25-1</f>
-        <v>295</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="2">
-        <v>32</v>
-      </c>
-      <c r="C26" s="2">
-        <f t="shared" si="10"/>
-        <v>296</v>
-      </c>
-      <c r="D26" s="2">
-        <f t="shared" si="11"/>
-        <v>327</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="2">
-        <v>5</v>
-      </c>
-      <c r="C27" s="2">
-        <f t="shared" si="10"/>
-        <v>328</v>
-      </c>
-      <c r="D27" s="2">
-        <f t="shared" si="11"/>
-        <v>332</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="B28" s="2">
         <v>32</v>
       </c>
       <c r="C28" s="2">
-        <f t="shared" si="10"/>
-        <v>333</v>
+        <f t="shared" si="12"/>
+        <v>264</v>
       </c>
       <c r="D28" s="2">
-        <f t="shared" si="11"/>
-        <v>364</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
+        <f t="shared" ref="D28:D49" si="13">B28+C28-1</f>
+        <v>295</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B29" s="2">
         <v>32</v>
       </c>
       <c r="C29" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
+        <v>296</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="13"/>
+        <v>327</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="2">
+        <v>5</v>
+      </c>
+      <c r="C30" s="2">
+        <f t="shared" si="12"/>
+        <v>328</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="13"/>
+        <v>332</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="2">
+        <v>32</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="12"/>
+        <v>333</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="13"/>
+        <v>364</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="2">
+        <v>32</v>
+      </c>
+      <c r="C32" s="2">
+        <f t="shared" si="12"/>
         <v>365</v>
       </c>
-      <c r="D29" s="2">
-        <f t="shared" si="11"/>
+      <c r="D32" s="2">
+        <f t="shared" si="13"/>
         <v>396</v>
       </c>
-      <c r="J29" s="3"/>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="2" t="s">
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B33" s="2">
         <v>32</v>
       </c>
-      <c r="C30" s="2">
-        <f t="shared" si="10"/>
+      <c r="C33" s="2">
+        <f t="shared" si="12"/>
         <v>397</v>
       </c>
-      <c r="D30" s="2">
-        <f t="shared" si="11"/>
+      <c r="D33" s="2">
+        <f t="shared" si="13"/>
         <v>428</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="7" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B34" s="7">
         <v>3</v>
       </c>
-      <c r="C31" s="7">
-        <f t="shared" si="10"/>
+      <c r="C34" s="7">
+        <f t="shared" si="12"/>
         <v>429</v>
       </c>
-      <c r="D31" s="7">
-        <f t="shared" si="11"/>
+      <c r="D34" s="7">
+        <f t="shared" si="13"/>
         <v>431</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="6" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B35" s="6">
         <v>1</v>
       </c>
-      <c r="C32" s="6">
-        <f t="shared" si="10"/>
+      <c r="C35" s="6">
+        <f t="shared" si="12"/>
         <v>432</v>
       </c>
-      <c r="D32" s="6">
-        <f t="shared" si="11"/>
+      <c r="D35" s="6">
+        <f t="shared" si="13"/>
         <v>432</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="4" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B36" s="4">
         <v>80</v>
       </c>
-      <c r="C33" s="4">
-        <f t="shared" si="10"/>
+      <c r="C36" s="4">
+        <f t="shared" si="12"/>
         <v>433</v>
       </c>
-      <c r="D33" s="4">
-        <f t="shared" si="11"/>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2">
-        <f t="shared" si="10"/>
-        <v>513</v>
-      </c>
-      <c r="D34" s="2">
-        <f t="shared" si="11"/>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2">
-        <f t="shared" si="10"/>
-        <v>513</v>
-      </c>
-      <c r="D35" s="2">
-        <f t="shared" si="11"/>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2">
-        <f t="shared" si="10"/>
-        <v>513</v>
-      </c>
-      <c r="D36" s="2">
-        <f t="shared" si="11"/>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="D36" s="4">
+        <f t="shared" si="13"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>513</v>
       </c>
       <c r="D37" s="2">
-        <f t="shared" si="11"/>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+        <f t="shared" si="13"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>513</v>
       </c>
       <c r="D38" s="2">
-        <f t="shared" si="11"/>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+        <f t="shared" si="13"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>513</v>
       </c>
       <c r="D39" s="2">
-        <f t="shared" si="11"/>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+        <f t="shared" si="13"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>513</v>
       </c>
       <c r="D40" s="2">
-        <f t="shared" si="11"/>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+        <f t="shared" si="13"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>513</v>
       </c>
       <c r="D41" s="2">
-        <f t="shared" si="11"/>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <f t="shared" si="13"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>513</v>
       </c>
       <c r="D42" s="2">
-        <f t="shared" si="11"/>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+        <f t="shared" si="13"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>513</v>
       </c>
       <c r="D43" s="2">
-        <f t="shared" si="11"/>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+        <f t="shared" si="13"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>513</v>
       </c>
       <c r="D44" s="2">
-        <f t="shared" si="11"/>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <f t="shared" si="13"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>513</v>
       </c>
       <c r="D45" s="2">
-        <f t="shared" si="11"/>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+        <f t="shared" si="13"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>513</v>
       </c>
       <c r="D46" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2">
+        <f t="shared" si="12"/>
+        <v>513</v>
+      </c>
+      <c r="D47" s="2">
+        <f t="shared" si="13"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2">
+        <f t="shared" si="12"/>
+        <v>513</v>
+      </c>
+      <c r="D48" s="2">
+        <f t="shared" si="13"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2">
+        <f t="shared" si="12"/>
+        <v>513</v>
+      </c>
+      <c r="D49" s="2">
+        <f t="shared" si="13"/>
         <v>512</v>
       </c>
     </row>

</xml_diff>